<commit_message>
further development of optimization
</commit_message>
<xml_diff>
--- a/input/c_matrix.xlsx
+++ b/input/c_matrix.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\02. Mestrado\TU Darmstadt\Energy Science and Engineering\5. Sommersemester 2023\Masterarbeit\5. Thesis\3. Python Routine\masterthesis\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C9137D-722B-4A20-8BFA-7C81136698B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD634EAD-8704-4D75-8886-FBB18E9BA8D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="conect" sheetId="1" r:id="rId1"/>
+    <sheet name="test" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="8">
   <si>
     <t>pv</t>
   </si>
@@ -40,6 +41,15 @@
   </si>
   <si>
     <t>from</t>
+  </si>
+  <si>
+    <t>quant_x</t>
+  </si>
+  <si>
+    <t>quant_y</t>
+  </si>
+  <si>
+    <t>quant_z</t>
   </si>
 </sst>
 </file>
@@ -359,8 +369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -454,4 +464,89 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F95E2386-39F3-4D2D-B0A8-D68B801DC43C}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
insert constraint generator on PVbat model
</commit_message>
<xml_diff>
--- a/input/c_matrix.xlsx
+++ b/input/c_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\02. Mestrado\TU Darmstadt\Energy Science and Engineering\5. Sommersemester 2023\Masterarbeit\5. Thesis\3. Python Routine\masterthesis\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8DB15A6-5943-4088-9ED3-78A9AB8E3939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC26327-2E7F-4B53-A0BD-E857F98A871E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -471,7 +471,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -512,10 +512,10 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">

</xml_diff>